<commit_message>
Update to sales terr
</commit_message>
<xml_diff>
--- a/Data/WingtipSalesRegions.xlsx
+++ b/Data/WingtipSalesRegions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Student\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PBI365\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Sales Regions" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,6 +428,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SalesRegions" displayName="SalesRegions" ref="A1:C51" totalsRowShown="0">
   <autoFilter ref="A1:C51"/>
+  <sortState ref="A2:C51">
+    <sortCondition ref="A1:A51"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="State"/>
     <tableColumn id="2" name="StateFullName" dataDxfId="0"/>
@@ -513,6 +516,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -548,6 +568,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -702,16 +739,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -722,51 +761,51 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -777,7 +816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -785,10 +824,10 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -799,7 +838,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -810,7 +849,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -821,7 +860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -832,7 +871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -843,51 +882,51 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -898,7 +937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -909,7 +948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -920,18 +959,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -942,18 +981,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -964,7 +1003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -975,29 +1014,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1008,95 +1047,95 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C34" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="C35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -1107,7 +1146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1118,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -1129,7 +1168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -1140,7 +1179,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -1151,7 +1190,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -1162,7 +1201,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -1173,7 +1212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -1184,7 +1223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -1195,7 +1234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -1206,29 +1245,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>92</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C46" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="C47" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -1239,29 +1278,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>98</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C49" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>100</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>102</v>
       </c>

</xml_diff>